<commit_message>
separa archivo por integrante
</commit_message>
<xml_diff>
--- a/Documentacion/Coevaluación.xlsx
+++ b/Documentacion/Coevaluación.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mt-my.sharepoint.com/personal/ptorres_metropolitan-touring_com/Documents/Documents/GitHub/PlataformaEventosUniversitarios/Documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB52DE9F-971C-41F1-9F8B-7AE37BC97166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{CB52DE9F-971C-41F1-9F8B-7AE37BC97166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E701C3E6-4C6C-459F-B477-AEC0BB63B940}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{91E3803E-7C67-4747-ABFD-5E3B8330F375}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Paul" sheetId="1" r:id="rId1"/>
+    <sheet name="Carlos" sheetId="2" r:id="rId2"/>
+    <sheet name="Jose" sheetId="3" r:id="rId3"/>
+    <sheet name="Kevin" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
   <si>
     <t>Estudiante</t>
   </si>
@@ -116,7 +119,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF202124"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -154,6 +176,98 @@
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF202124"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF202124"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF202124"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF202124"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF202124"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -168,15 +282,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CE45D74-80FA-4222-B91B-BB4B9971F95E}" name="Tabla1" displayName="Tabla1" ref="A1:F5" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:F5" xr:uid="{3CE45D74-80FA-4222-B91B-BB4B9971F95E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CE45D74-80FA-4222-B91B-BB4B9971F95E}" name="Tabla1" displayName="Tabla1" ref="A1:F4" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:F4" xr:uid="{3CE45D74-80FA-4222-B91B-BB4B9971F95E}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{BCDE5B52-BC5B-475D-9A48-6F9FDB10A28D}" name="Estudiante" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{BCDE5B52-BC5B-475D-9A48-6F9FDB10A28D}" name="Estudiante" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{8260A236-5A6F-45D7-A9E6-FD81914B4F52}" name="Asistencia a reuniones, cumplimiento de tareas, actitud proactiva."/>
     <tableColumn id="3" xr3:uid="{6E303590-759F-4BC4-97FF-F6D706210394}" name="Calidad del trabajo técnico aportado (código, diagramas, ideas de diseño)."/>
     <tableColumn id="4" xr3:uid="{284B97B2-B30F-48EB-B897-7DC4F5706EB1}" name="Uso efectivo de ramas, commits claros, participación en revisiones."/>
     <tableColumn id="5" xr3:uid="{AA2A8EBE-D46B-4CCD-9244-C1D079837FF7}" name="Claridad para explicar ideas, receptividad al feedback, coordinación con el equipo."/>
     <tableColumn id="6" xr3:uid="{EF30F9ED-3AB5-4679-9D2F-D0BDDCD5CE6A}" name="Entregas puntuales, cumplimiento de acuerdos, autonomía."/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2BD79B2D-AE84-4A3C-A67B-51B5857B1200}" name="Tabla13" displayName="Tabla13" ref="A1:F4" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F4" xr:uid="{3CE45D74-80FA-4222-B91B-BB4B9971F95E}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{985B324D-6F29-462B-A896-9A13A82835D8}" name="Estudiante" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{39073BDD-BE96-488F-B58F-6CCF8B3378AB}" name="Asistencia a reuniones, cumplimiento de tareas, actitud proactiva."/>
+    <tableColumn id="3" xr3:uid="{5E464D0B-9F58-46DB-94AF-C4A558B5DDFE}" name="Calidad del trabajo técnico aportado (código, diagramas, ideas de diseño)."/>
+    <tableColumn id="4" xr3:uid="{3D84F728-F67B-4A86-B56F-01E6320F6A53}" name="Uso efectivo de ramas, commits claros, participación en revisiones."/>
+    <tableColumn id="5" xr3:uid="{C883F4B5-CA15-479E-A006-117B3BAECD0C}" name="Claridad para explicar ideas, receptividad al feedback, coordinación con el equipo."/>
+    <tableColumn id="6" xr3:uid="{5A6CD665-7187-4693-8E3E-E0AE10612130}" name="Entregas puntuales, cumplimiento de acuerdos, autonomía."/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3181C7D2-8427-47AB-B136-6E695F4CF784}" name="Tabla134" displayName="Tabla134" ref="A1:F4" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:F4" xr:uid="{3CE45D74-80FA-4222-B91B-BB4B9971F95E}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{2EC7B2B4-B531-4290-9D07-7FFA67F51145}" name="Estudiante" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{85883107-9D9F-40ED-A21E-335151666C57}" name="Asistencia a reuniones, cumplimiento de tareas, actitud proactiva."/>
+    <tableColumn id="3" xr3:uid="{33FBCB2D-F73A-4D89-83C8-8B2259EAF1D0}" name="Calidad del trabajo técnico aportado (código, diagramas, ideas de diseño)."/>
+    <tableColumn id="4" xr3:uid="{D62E9875-654C-4F46-AA97-EA7BD538A6B4}" name="Uso efectivo de ramas, commits claros, participación en revisiones."/>
+    <tableColumn id="5" xr3:uid="{6150C667-E33C-421E-BE4B-0265A05E6691}" name="Claridad para explicar ideas, receptividad al feedback, coordinación con el equipo."/>
+    <tableColumn id="6" xr3:uid="{052E184F-A174-45A6-B08D-E3173E6F0B2F}" name="Entregas puntuales, cumplimiento de acuerdos, autonomía."/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1DA7592F-C9EA-4ECD-8F16-8FDD94012FF8}" name="Tabla1345" displayName="Tabla1345" ref="A1:F4" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:F4" xr:uid="{3CE45D74-80FA-4222-B91B-BB4B9971F95E}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{3C31C65E-A899-440D-B3CF-4E181D5A0A2B}" name="Estudiante" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{98334846-3B92-4AF1-AD28-D220F140F56C}" name="Asistencia a reuniones, cumplimiento de tareas, actitud proactiva."/>
+    <tableColumn id="3" xr3:uid="{766DC799-E11C-4240-8288-D537A0D3E264}" name="Calidad del trabajo técnico aportado (código, diagramas, ideas de diseño)."/>
+    <tableColumn id="4" xr3:uid="{5025DEE9-FCEB-4879-9B0A-FBDEADAB33A1}" name="Uso efectivo de ramas, commits claros, participación en revisiones."/>
+    <tableColumn id="5" xr3:uid="{EBF9F625-E8E5-479A-A608-30F925161008}" name="Claridad para explicar ideas, receptividad al feedback, coordinación con el equipo."/>
+    <tableColumn id="6" xr3:uid="{056DA4CF-6E19-4EF1-9D46-7474629AE226}" name="Entregas puntuales, cumplimiento de acuerdos, autonomía."/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -499,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92AA2862-2667-455A-850C-7A5C3E12FEF5}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,12 +706,190 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C6A51B-EDF1-4B98-8C75-64CAD7D998BE}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.109375" customWidth="1"/>
+    <col min="5" max="5" width="69.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CE66F4-F106-4A26-8248-30A8401D5FAC}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.109375" customWidth="1"/>
+    <col min="5" max="5" width="69.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EFDDC2-677F-400D-A53C-8C0E769DB13F}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.109375" customWidth="1"/>
+    <col min="5" max="5" width="69.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>